<commit_message>
-commit update terakhir 01-09-2015
</commit_message>
<xml_diff>
--- a/file/rekap_reformasi_kesehatan.xlsx
+++ b/file/rekap_reformasi_kesehatan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sikkes\file\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="8445"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>NO</t>
   </si>
@@ -55,9 +60,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Reform 1. Pengembangan</t>
@@ -87,11 +89,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,12 +137,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -264,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -308,21 +304,6 @@
     </xf>
     <xf numFmtId="41" fontId="1" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -345,6 +326,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -391,7 +380,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,9 +412,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,6 +447,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -632,14 +623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="37" style="4" customWidth="1"/>
@@ -662,113 +653,113 @@
     <col min="19" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75">
-      <c r="A1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-    </row>
-    <row r="2" spans="1:19" ht="18.75" customHeight="1"/>
-    <row r="3" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A3" s="25" t="s">
+    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+    </row>
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="24"/>
-    </row>
-    <row r="4" spans="1:19" ht="30.75" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="19"/>
+    </row>
+    <row r="4" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -789,7 +780,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="13"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -810,7 +801,7 @@
       <c r="R6" s="14"/>
       <c r="S6" s="15"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -831,7 +822,7 @@
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -852,7 +843,7 @@
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -873,7 +864,7 @@
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -894,7 +885,7 @@
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -915,7 +906,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -936,7 +927,7 @@
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -957,7 +948,7 @@
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -978,7 +969,7 @@
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -999,221 +990,8 @@
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
     </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="15"/>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="15"/>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="15"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="15"/>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="15"/>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="15"/>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="15"/>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="15"/>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="15"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1">
-      <c r="A25" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="17"/>
-    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A25:K25"/>
+  <mergeCells count="13">
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="L3:S3"/>
     <mergeCell ref="G3:G4"/>
@@ -1234,24 +1012,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>